<commit_message>
Added new table userInfo to handle case where one employee may work at multiple locations and or have multiple roles. Still a blind commit, must be tested in vm.
</commit_message>
<xml_diff>
--- a/project01/tavernDB_plan.xlsx
+++ b/project01/tavernDB_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wlgro\Documents\MTwdbc\project01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9C4314-3F20-426E-8896-2CD7FC136693}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4BA7AE-8F7A-4588-9E9E-4C3E6ADDF232}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C740F7E-A40E-4004-A829-37DED4AD7C50}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>taverns</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Version: 1.0</t>
+  </si>
+  <si>
+    <t>userInfo</t>
+  </si>
+  <si>
+    <t>user_ID*</t>
   </si>
 </sst>
 </file>
@@ -212,24 +218,6 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
       <border>
         <bottom style="medium">
           <color indexed="64"/>
@@ -264,6 +252,24 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -278,7 +284,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7096E7D1-F8E7-419E-BD8C-EF19C45FCC72}" name="Table1" displayName="Table1" ref="C7:C9" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7096E7D1-F8E7-419E-BD8C-EF19C45FCC72}" name="Table1" displayName="Table1" ref="C7:C9" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4">
   <autoFilter ref="C7:C9" xr:uid="{2C7932CE-DFF9-4DE4-8660-236CC538172C}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{BDC645B2-19E1-4193-BD52-56EA3CF4283D}" name="taverns"/>
@@ -288,8 +294,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{46711480-114A-4681-83F1-8DE6D0E58D93}" name="Table2" displayName="Table2" ref="E7:E10" totalsRowShown="0" headerRowBorderDxfId="4">
-  <autoFilter ref="E7:E10" xr:uid="{DA1D9047-FC83-486D-BD7A-FC320A46401B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{46711480-114A-4681-83F1-8DE6D0E58D93}" name="Table2" displayName="Table2" ref="G7:G10" totalsRowShown="0" headerRowBorderDxfId="3">
+  <autoFilter ref="G7:G10" xr:uid="{DA1D9047-FC83-486D-BD7A-FC320A46401B}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{F9DC3A60-FD7B-4229-84F2-0F4E58212DCF}" name="roles"/>
   </tableColumns>
@@ -298,18 +304,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FC064323-5FE6-44DE-A344-11F2ED4F40C8}" name="Table3" displayName="Table3" ref="G7:G14" totalsRowShown="0" headerRowBorderDxfId="5">
-  <autoFilter ref="G7:G14" xr:uid="{19AA1E90-698E-4681-BBB1-3EBB1093974C}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{9B61F9A7-08D3-4AB0-84D8-3D601F70445F}" name="locations"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5A8D7824-75B9-4AEC-BC4C-2FF67EB24AC6}" name="Table4" displayName="Table4" ref="I7:I11" totalsRowShown="0" headerRowBorderDxfId="2">
-  <autoFilter ref="I7:I11" xr:uid="{0009006E-F2BE-49EC-9B9C-89DAA3221E82}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5A8D7824-75B9-4AEC-BC4C-2FF67EB24AC6}" name="Table4" displayName="Table4" ref="E7:E9" totalsRowShown="0" headerRowBorderDxfId="2">
+  <autoFilter ref="E7:E9" xr:uid="{0009006E-F2BE-49EC-9B9C-89DAA3221E82}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{40ED2253-283F-4C54-9CCD-CDF5E45F2527}" name="users"/>
   </tableColumns>
@@ -317,7 +313,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A6045E39-8167-4CFF-9682-697F82ACC587}" name="Table5" displayName="Table5" ref="K7:K10" totalsRowShown="0" headerRowBorderDxfId="1">
   <autoFilter ref="K7:K10" xr:uid="{C3767C89-8AFD-468D-A0C0-777950FB6ACE}"/>
   <tableColumns count="1">
@@ -327,13 +323,33 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3899325B-595E-416D-9999-73ACC4EC1845}" name="Table6" displayName="Table6" ref="A7:A10" totalsRowShown="0">
   <autoFilter ref="A7:A10" xr:uid="{4BB83632-76C7-47B8-A82E-9D4360E356ED}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{43962FE2-38D2-4CF2-A2BC-ED1581C8B51E}" name="KEY (not representative of a table in the DB)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9FE0EB35-79A4-4DFC-9119-7B9E221EE218}" name="Table7" displayName="Table7" ref="M7:M10" totalsRowShown="0">
+  <autoFilter ref="M7:M10" xr:uid="{88D9DDB3-F95C-48D6-8F90-82D0A9B085DE}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{4104F8A5-14A9-4402-9B3E-0858EDCB6101}" name="userInfo"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B424434C-92D3-4766-B20A-FE9BEBA7CC29}" name="Table39" displayName="Table39" ref="I7:I14" totalsRowShown="0" headerRowBorderDxfId="0">
+  <autoFilter ref="I7:I14" xr:uid="{09E8337E-8920-46B5-A10B-CC0EE69AF291}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{4A750CEF-BB89-4295-84BD-46EDBCA0B20E}" name="locations"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -634,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED40847-C0F9-4BC0-A326-1C1410336474}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,36 +662,37 @@
     <col min="3" max="3" width="9.109375" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -683,39 +700,45 @@
         <v>0</v>
       </c>
       <c r="E7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="I7" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>7</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>2</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M8" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -723,68 +746,69 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
         <v>4</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>9</v>
-      </c>
-      <c r="I9" t="s">
-        <v>1</v>
       </c>
       <c r="K9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>5</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>10</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G11" t="s">
+      <c r="M10" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G12" t="s">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G13" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G14" s="1" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I14" s="1" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-  <tableParts count="6">
+  <tableParts count="7">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New DB plan based on revised requirements
</commit_message>
<xml_diff>
--- a/project01/tavernDB_plan.xlsx
+++ b/project01/tavernDB_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wlgro\Documents\MTwdbc\project01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4BA7AE-8F7A-4588-9E9E-4C3E6ADDF232}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E62ED67-366A-4E75-852B-5B1964F06556}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C740F7E-A40E-4004-A829-37DED4AD7C50}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
   <si>
     <t>taverns</t>
   </si>
@@ -115,6 +115,60 @@
   </si>
   <si>
     <t>user_ID*</t>
+  </si>
+  <si>
+    <t>guests</t>
+  </si>
+  <si>
+    <t>supplies</t>
+  </si>
+  <si>
+    <t>services</t>
+  </si>
+  <si>
+    <t>statuses</t>
+  </si>
+  <si>
+    <t>service statuses</t>
+  </si>
+  <si>
+    <t>inventory</t>
+  </si>
+  <si>
+    <t>orders</t>
+  </si>
+  <si>
+    <t>sales</t>
+  </si>
+  <si>
+    <t>birthday</t>
+  </si>
+  <si>
+    <t>service_ID*</t>
+  </si>
+  <si>
+    <t>status_ID*</t>
+  </si>
+  <si>
+    <t>supply_ID*</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>guest_ID*</t>
+  </si>
+  <si>
+    <t>price</t>
   </si>
 </sst>
 </file>
@@ -130,6 +184,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -137,7 +192,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,8 +235,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -198,11 +277,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -211,12 +333,29 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <bottom style="medium">
@@ -284,7 +423,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7096E7D1-F8E7-419E-BD8C-EF19C45FCC72}" name="Table1" displayName="Table1" ref="C7:C9" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7096E7D1-F8E7-419E-BD8C-EF19C45FCC72}" name="Table1" displayName="Table1" ref="C7:C9" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5">
   <autoFilter ref="C7:C9" xr:uid="{2C7932CE-DFF9-4DE4-8660-236CC538172C}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{BDC645B2-19E1-4193-BD52-56EA3CF4283D}" name="taverns"/>
@@ -293,9 +432,39 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C8A11E63-AC69-4A73-A659-95A28A41EB5D}" name="Table11" displayName="Table11" ref="K17:K23" totalsRowShown="0">
+  <autoFilter ref="K17:K23" xr:uid="{071116D3-29E3-47D1-AA51-D708F7ADB922}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{9377DE04-38AE-4703-9465-C1D34F281DD3}" name="inventory"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{E0313658-BE98-44C4-A5EF-E85C335A6F08}" name="Table12" displayName="Table12" ref="M17:M24" totalsRowShown="0">
+  <autoFilter ref="M17:M24" xr:uid="{652B734C-A0CD-419C-B888-F23686DB823B}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{DBA2D4E4-53FE-4E83-8711-5754E4E4E11C}" name="orders"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{4F2C4954-8A20-4486-BE7E-0C84415CE640}" name="Table13" displayName="Table13" ref="O17:O24" totalsRowShown="0">
+  <autoFilter ref="O17:O24" xr:uid="{57054837-248C-435C-81CC-5C24885158EC}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{EE19AD34-4EE5-44BD-91A0-2CAA588F520F}" name="sales"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{46711480-114A-4681-83F1-8DE6D0E58D93}" name="Table2" displayName="Table2" ref="G7:G10" totalsRowShown="0" headerRowBorderDxfId="3">
-  <autoFilter ref="G7:G10" xr:uid="{DA1D9047-FC83-486D-BD7A-FC320A46401B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{46711480-114A-4681-83F1-8DE6D0E58D93}" name="Table2" displayName="Table2" ref="I7:I10" totalsRowShown="0" headerRowBorderDxfId="4">
+  <autoFilter ref="I7:I10" xr:uid="{DA1D9047-FC83-486D-BD7A-FC320A46401B}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{F9DC3A60-FD7B-4229-84F2-0F4E58212DCF}" name="roles"/>
   </tableColumns>
@@ -304,7 +473,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5A8D7824-75B9-4AEC-BC4C-2FF67EB24AC6}" name="Table4" displayName="Table4" ref="E7:E9" totalsRowShown="0" headerRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5A8D7824-75B9-4AEC-BC4C-2FF67EB24AC6}" name="Table4" displayName="Table4" ref="E7:E9" totalsRowShown="0" headerRowBorderDxfId="3">
   <autoFilter ref="E7:E9" xr:uid="{0009006E-F2BE-49EC-9B9C-89DAA3221E82}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{40ED2253-283F-4C54-9CCD-CDF5E45F2527}" name="users"/>
@@ -314,12 +483,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A6045E39-8167-4CFF-9682-697F82ACC587}" name="Table5" displayName="Table5" ref="K7:K10" totalsRowShown="0" headerRowBorderDxfId="1">
-  <autoFilter ref="K7:K10" xr:uid="{C3767C89-8AFD-468D-A0C0-777950FB6ACE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A6045E39-8167-4CFF-9682-697F82ACC587}" name="Table5" displayName="Table5" ref="M7:M10" totalsRowShown="0" headerRowBorderDxfId="2">
+  <autoFilter ref="M7:M10" xr:uid="{C3767C89-8AFD-468D-A0C0-777950FB6ACE}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{9D94D518-D861-4C83-9DD7-51702D2EBD67}" name="rats"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -334,8 +503,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9FE0EB35-79A4-4DFC-9119-7B9E221EE218}" name="Table7" displayName="Table7" ref="M7:M10" totalsRowShown="0">
-  <autoFilter ref="M7:M10" xr:uid="{88D9DDB3-F95C-48D6-8F90-82D0A9B085DE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9FE0EB35-79A4-4DFC-9119-7B9E221EE218}" name="Table7" displayName="Table7" ref="O7:O10" totalsRowShown="0">
+  <autoFilter ref="O7:O10" xr:uid="{88D9DDB3-F95C-48D6-8F90-82D0A9B085DE}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{4104F8A5-14A9-4402-9B3E-0858EDCB6101}" name="userInfo"/>
   </tableColumns>
@@ -344,12 +513,32 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B424434C-92D3-4766-B20A-FE9BEBA7CC29}" name="Table39" displayName="Table39" ref="I7:I14" totalsRowShown="0" headerRowBorderDxfId="0">
-  <autoFilter ref="I7:I14" xr:uid="{09E8337E-8920-46B5-A10B-CC0EE69AF291}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B424434C-92D3-4766-B20A-FE9BEBA7CC29}" name="Table39" displayName="Table39" ref="K7:K14" totalsRowShown="0" headerRowBorderDxfId="1">
+  <autoFilter ref="K7:K14" xr:uid="{09E8337E-8920-46B5-A10B-CC0EE69AF291}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{4A750CEF-BB89-4295-84BD-46EDBCA0B20E}" name="locations"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{90DD2A3B-9B2F-4E7F-AE80-5AC149959B78}" name="Table3" displayName="Table3" ref="G7:G10" totalsRowShown="0" headerRowBorderDxfId="0">
+  <autoFilter ref="G7:G10" xr:uid="{57E399F1-F9D4-4D4C-8469-C8EF0893DB21}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{7C79CAA0-5975-4B3A-A81B-E499F733901E}" name="guests"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{40C79247-19A0-4E0B-84A5-473408D59042}" name="Table10" displayName="Table10" ref="I17:I20" totalsRowShown="0">
+  <autoFilter ref="I17:I20" xr:uid="{9823955D-61C9-4EEB-A512-F5F779D89F01}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{5CD34190-B481-4F09-B449-551A4F609BD5}" name="service statuses"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -650,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED40847-C0F9-4BC0-A326-1C1410336474}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,60 +851,64 @@
     <col min="3" max="3" width="9.109375" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="M7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -725,20 +918,23 @@
       <c r="E8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -749,59 +945,189 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
         <v>4</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>9</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>1</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="G10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" t="s">
         <v>5</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>10</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I11" t="s">
+      <c r="O10" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I12" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I13" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I14" s="1" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K14" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" t="s">
+        <v>34</v>
+      </c>
+      <c r="O17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C18" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" t="s">
+        <v>2</v>
+      </c>
+      <c r="O18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C19" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="I20" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="O20" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="K21" t="s">
+        <v>40</v>
+      </c>
+      <c r="M21" t="s">
+        <v>40</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="K22" t="s">
+        <v>41</v>
+      </c>
+      <c r="M22" t="s">
+        <v>41</v>
+      </c>
+      <c r="O22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="K23" t="s">
+        <v>42</v>
+      </c>
+      <c r="M23" t="s">
+        <v>43</v>
+      </c>
+      <c r="O23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="M24" t="s">
+        <v>42</v>
+      </c>
+      <c r="O24" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-  <tableParts count="7">
+  <tableParts count="12">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -809,6 +1135,11 @@
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
further modified db plan, updated script to match new plan, script still not tested
</commit_message>
<xml_diff>
--- a/project01/tavernDB_plan.xlsx
+++ b/project01/tavernDB_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wlgro\Documents\MTwdbc\project01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E62ED67-366A-4E75-852B-5B1964F06556}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66595D6-5ADC-4833-B65E-9696B9845FE5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C740F7E-A40E-4004-A829-37DED4AD7C50}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="49">
   <si>
     <t>taverns</t>
   </si>
@@ -129,9 +129,6 @@
     <t>statuses</t>
   </si>
   <si>
-    <t>service statuses</t>
-  </si>
-  <si>
     <t>inventory</t>
   </si>
   <si>
@@ -169,6 +166,18 @@
   </si>
   <si>
     <t>price</t>
+  </si>
+  <si>
+    <t>serviceStatuses</t>
+  </si>
+  <si>
+    <t>serviceSupplies</t>
+  </si>
+  <si>
+    <t>unit_ID*</t>
+  </si>
+  <si>
+    <t>Notes:                                                                              serviceSupplies and serviceStatuses could be merged if an entry can lack a supply ID and/or count and not break the db (for services like pool where no supplies are being depleted)</t>
   </si>
 </sst>
 </file>
@@ -192,7 +201,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +265,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF51C9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -324,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -344,6 +359,12 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,6 +432,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF51C9"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -433,8 +459,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C8A11E63-AC69-4A73-A659-95A28A41EB5D}" name="Table11" displayName="Table11" ref="K17:K23" totalsRowShown="0">
-  <autoFilter ref="K17:K23" xr:uid="{071116D3-29E3-47D1-AA51-D708F7ADB922}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C8A11E63-AC69-4A73-A659-95A28A41EB5D}" name="Table11" displayName="Table11" ref="I13:I19" totalsRowShown="0">
+  <autoFilter ref="I13:I19" xr:uid="{071116D3-29E3-47D1-AA51-D708F7ADB922}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{9377DE04-38AE-4703-9465-C1D34F281DD3}" name="inventory"/>
   </tableColumns>
@@ -443,8 +469,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{E0313658-BE98-44C4-A5EF-E85C335A6F08}" name="Table12" displayName="Table12" ref="M17:M24" totalsRowShown="0">
-  <autoFilter ref="M17:M24" xr:uid="{652B734C-A0CD-419C-B888-F23686DB823B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{E0313658-BE98-44C4-A5EF-E85C335A6F08}" name="Table12" displayName="Table12" ref="K13:K20" totalsRowShown="0">
+  <autoFilter ref="K13:K20" xr:uid="{652B734C-A0CD-419C-B888-F23686DB823B}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{DBA2D4E4-53FE-4E83-8711-5754E4E4E11C}" name="orders"/>
   </tableColumns>
@@ -453,10 +479,20 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{4F2C4954-8A20-4486-BE7E-0C84415CE640}" name="Table13" displayName="Table13" ref="O17:O24" totalsRowShown="0">
-  <autoFilter ref="O17:O24" xr:uid="{57054837-248C-435C-81CC-5C24885158EC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{4F2C4954-8A20-4486-BE7E-0C84415CE640}" name="Table13" displayName="Table13" ref="M13:M19" totalsRowShown="0">
+  <autoFilter ref="M13:M19" xr:uid="{57054837-248C-435C-81CC-5C24885158EC}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{EE19AD34-4EE5-44BD-91A0-2CAA588F520F}" name="sales"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4CB56E77-DF6D-4104-88AD-577CB2EE4243}" name="Table9" displayName="Table9" ref="O13:O18" totalsRowShown="0">
+  <autoFilter ref="O13:O18" xr:uid="{DCB6CCE4-7913-4438-ABF2-BF1065BDB3C8}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{D29CD843-3E38-4C53-8220-E290B9F7AD62}" name="serviceSupplies"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -483,8 +519,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A6045E39-8167-4CFF-9682-697F82ACC587}" name="Table5" displayName="Table5" ref="M7:M10" totalsRowShown="0" headerRowBorderDxfId="2">
-  <autoFilter ref="M7:M10" xr:uid="{C3767C89-8AFD-468D-A0C0-777950FB6ACE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A6045E39-8167-4CFF-9682-697F82ACC587}" name="Table5" displayName="Table5" ref="G13:G16" totalsRowShown="0" headerRowBorderDxfId="2">
+  <autoFilter ref="G13:G16" xr:uid="{C3767C89-8AFD-468D-A0C0-777950FB6ACE}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{9D94D518-D861-4C83-9DD7-51702D2EBD67}" name="rats"/>
   </tableColumns>
@@ -503,8 +539,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9FE0EB35-79A4-4DFC-9119-7B9E221EE218}" name="Table7" displayName="Table7" ref="O7:O10" totalsRowShown="0">
-  <autoFilter ref="O7:O10" xr:uid="{88D9DDB3-F95C-48D6-8F90-82D0A9B085DE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9FE0EB35-79A4-4DFC-9119-7B9E221EE218}" name="Table7" displayName="Table7" ref="E23:E26" totalsRowShown="0">
+  <autoFilter ref="E23:E26" xr:uid="{88D9DDB3-F95C-48D6-8F90-82D0A9B085DE}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{4104F8A5-14A9-4402-9B3E-0858EDCB6101}" name="userInfo"/>
   </tableColumns>
@@ -513,8 +549,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B424434C-92D3-4766-B20A-FE9BEBA7CC29}" name="Table39" displayName="Table39" ref="K7:K14" totalsRowShown="0" headerRowBorderDxfId="1">
-  <autoFilter ref="K7:K14" xr:uid="{09E8337E-8920-46B5-A10B-CC0EE69AF291}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B424434C-92D3-4766-B20A-FE9BEBA7CC29}" name="Table39" displayName="Table39" ref="E13:E20" totalsRowShown="0" headerRowBorderDxfId="1">
+  <autoFilter ref="E13:E20" xr:uid="{09E8337E-8920-46B5-A10B-CC0EE69AF291}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{4A750CEF-BB89-4295-84BD-46EDBCA0B20E}" name="locations"/>
   </tableColumns>
@@ -533,10 +569,10 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{40C79247-19A0-4E0B-84A5-473408D59042}" name="Table10" displayName="Table10" ref="I17:I20" totalsRowShown="0">
-  <autoFilter ref="I17:I20" xr:uid="{9823955D-61C9-4EEB-A512-F5F779D89F01}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{40C79247-19A0-4E0B-84A5-473408D59042}" name="Table10" displayName="Table10" ref="C23:C27" totalsRowShown="0">
+  <autoFilter ref="C23:C27" xr:uid="{9823955D-61C9-4EEB-A512-F5F779D89F01}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{5CD34190-B481-4F09-B449-551A4F609BD5}" name="service statuses"/>
+    <tableColumn id="1" xr3:uid="{5CD34190-B481-4F09-B449-551A4F609BD5}" name="serviceStatuses"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -839,22 +875,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED40847-C0F9-4BC0-A326-1C1410336474}">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -898,14 +934,14 @@
       <c r="I7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="O7" t="s">
-        <v>26</v>
+      <c r="K7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="18" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -924,14 +960,14 @@
       <c r="I8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="M8" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="O8" s="4" t="s">
-        <v>27</v>
+      <c r="O8" s="13" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -950,14 +986,14 @@
       <c r="I9" t="s">
         <v>4</v>
       </c>
-      <c r="K9" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="K9" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>15</v>
+      <c r="M9" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -965,169 +1001,225 @@
         <v>19</v>
       </c>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I10" t="s">
         <v>5</v>
       </c>
-      <c r="K10" t="s">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="22"/>
+      <c r="C13" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" t="s">
+        <v>34</v>
+      </c>
+      <c r="O13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="22"/>
+      <c r="C14" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" t="s">
+        <v>2</v>
+      </c>
+      <c r="M14" t="s">
+        <v>2</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="22"/>
+      <c r="C15" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="22"/>
+      <c r="E16" t="s">
         <v>10</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="5" t="s">
+      <c r="I16" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="22"/>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" t="s">
+        <v>39</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="22"/>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="M18" t="s">
+        <v>39</v>
+      </c>
+      <c r="O18" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="22"/>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" t="s">
+        <v>41</v>
+      </c>
+      <c r="K19" t="s">
+        <v>42</v>
+      </c>
+      <c r="M19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="22"/>
+      <c r="E20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="22"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="22"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="22"/>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="22"/>
+      <c r="C24" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K14" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" t="s">
-        <v>32</v>
-      </c>
-      <c r="K17" t="s">
-        <v>33</v>
-      </c>
-      <c r="M17" t="s">
-        <v>34</v>
-      </c>
-      <c r="O17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C18" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="I18" s="5" t="s">
+      <c r="E24" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="22"/>
+      <c r="C25" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="22"/>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K18" t="s">
-        <v>2</v>
-      </c>
-      <c r="M18" t="s">
-        <v>2</v>
-      </c>
-      <c r="O18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C19" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="I19" s="10" t="s">
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="22"/>
+      <c r="C27" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O19" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="I20" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="M20" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="O20" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="K21" t="s">
-        <v>40</v>
-      </c>
-      <c r="M21" t="s">
-        <v>40</v>
-      </c>
-      <c r="O21" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="K22" t="s">
-        <v>41</v>
-      </c>
-      <c r="M22" t="s">
-        <v>41</v>
-      </c>
-      <c r="O22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="K23" t="s">
-        <v>42</v>
-      </c>
-      <c r="M23" t="s">
-        <v>43</v>
-      </c>
-      <c r="O23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="M24" t="s">
-        <v>42</v>
-      </c>
-      <c r="O24" t="s">
-        <v>42</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A12:A27"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-  <tableParts count="12">
+  <tableParts count="13">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -1140,6 +1232,7 @@
     <tablePart r:id="rId11"/>
     <tablePart r:id="rId12"/>
     <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>